<commit_message>
Fix variable naming in tests
</commit_message>
<xml_diff>
--- a/tests/input/4kp50.xlsx
+++ b/tests/input/4kp50.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\whbles\pyaugmecon\tests\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD588AF5-9D3B-43D8-99EE-1DACE088C25E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124732B2-A2C9-4BC3-B312-8C4FA83E48F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="3465" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{DF6384DB-DFB1-4F3E-A725-F1DA5E529D8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{DF6384DB-DFB1-4F3E-A725-F1DA5E529D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
@@ -2027,7 +2027,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="G2:K5"/>
+      <selection activeCell="H14" sqref="A6:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,16 +2051,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>269</v>
+        <v>782</v>
       </c>
       <c r="C2">
-        <v>196</v>
+        <v>755</v>
       </c>
       <c r="D2">
-        <v>134</v>
+        <v>744</v>
       </c>
       <c r="E2">
-        <v>163</v>
+        <v>718</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2068,16 +2068,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>168</v>
+        <v>743</v>
       </c>
       <c r="C3">
-        <v>278</v>
+        <v>770</v>
       </c>
       <c r="D3">
-        <v>159</v>
+        <v>728</v>
       </c>
       <c r="E3">
-        <v>157</v>
+        <v>727</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2085,16 +2085,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>171</v>
+        <v>739</v>
       </c>
       <c r="C4">
-        <v>209</v>
+        <v>746</v>
       </c>
       <c r="D4">
-        <v>246</v>
+        <v>769</v>
       </c>
       <c r="E4">
-        <v>193</v>
+        <v>725</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2102,16 +2102,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>152</v>
+        <v>727</v>
       </c>
       <c r="C5">
-        <v>172</v>
+        <v>741</v>
       </c>
       <c r="D5">
-        <v>146</v>
+        <v>735</v>
       </c>
       <c r="E5">
-        <v>261</v>
+        <v>757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Round test solutions before sorting to correctly assert arrays
</commit_message>
<xml_diff>
--- a/tests/input/4kp50.xlsx
+++ b/tests/input/4kp50.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\whbles\pyaugmecon\tests\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E37A6A7-E627-4EA8-9CD0-663645A81A11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDB17DB-64F4-4EBF-88EA-CD00C70823AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{DF6384DB-DFB1-4F3E-A725-F1DA5E529D8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{DF6384DB-DFB1-4F3E-A725-F1DA5E529D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
     <sheet name="b" sheetId="2" r:id="rId2"/>
     <sheet name="c" sheetId="3" r:id="rId3"/>
     <sheet name="payoff_table" sheetId="5" r:id="rId4"/>
-    <sheet name="e_points" sheetId="6" r:id="rId5"/>
-    <sheet name="pareto_sols" sheetId="4" r:id="rId6"/>
+    <sheet name="pareto_sols" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -395,7 +394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DC46A5-267B-4B7C-90B0-800E9C85533E}">
   <dimension ref="A1:AY5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -2020,15 +2019,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0071402-2D78-4181-BB21-3DE3215638CB}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:P5"/>
+      <selection activeCell="K5" sqref="F1:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1</v>
       </c>
@@ -2042,7 +2041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2058,20 +2057,8 @@
       <c r="E2">
         <v>718</v>
       </c>
-      <c r="H2">
-        <v>782</v>
-      </c>
-      <c r="I2">
-        <v>755</v>
-      </c>
-      <c r="J2">
-        <v>744</v>
-      </c>
-      <c r="K2">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2087,20 +2074,8 @@
       <c r="E3">
         <v>727</v>
       </c>
-      <c r="H3">
-        <v>743</v>
-      </c>
-      <c r="I3">
-        <v>770</v>
-      </c>
-      <c r="J3">
-        <v>728</v>
-      </c>
-      <c r="K3">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2116,20 +2091,8 @@
       <c r="E4">
         <v>725</v>
       </c>
-      <c r="H4">
-        <v>739</v>
-      </c>
-      <c r="I4">
-        <v>746</v>
-      </c>
-      <c r="J4">
-        <v>769</v>
-      </c>
-      <c r="K4">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2143,18 +2106,6 @@
         <v>735</v>
       </c>
       <c r="E5">
-        <v>757</v>
-      </c>
-      <c r="H5">
-        <v>727</v>
-      </c>
-      <c r="I5">
-        <v>741</v>
-      </c>
-      <c r="J5">
-        <v>735</v>
-      </c>
-      <c r="K5">
         <v>757</v>
       </c>
     </row>
@@ -2164,25 +2115,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B980400-298C-4B39-911D-DEEE2CE3B997}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831A6850-8724-4B70-A817-487B45869133}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:J1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>